<commit_message>
updated the impedance dataset for all subjects
</commit_message>
<xml_diff>
--- a/dataset/impedance_frequency_sweep/54.xlsx
+++ b/dataset/impedance_frequency_sweep/54.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\My Drive\Professional\Academic\Postdoc\Projects\Impedance\data\patients data\palmsense files Jan 2025\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mac\Home\Documents\GitHubs\postdoc\wound_EHR_analyzer_private\dataset\impedance_frequency_sweep\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FFBB888-E8E6-4CAF-BE48-2280378EA39E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{85BBBBA8-83A7-495C-869C-04724584BAE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="420" yWindow="7658" windowWidth="20168" windowHeight="11850" activeTab="1" xr2:uid="{7A0F474E-1994-4708-A8DE-2B4D2CC6525B}"/>
+    <workbookView xWindow="735" yWindow="1110" windowWidth="31335" windowHeight="17190" xr2:uid="{B329B19D-4732-442B-87A7-97DD20E85021}"/>
   </bookViews>
   <sheets>
-    <sheet name="54_visit_3 0.9" sheetId="3" r:id="rId1"/>
-    <sheet name="54_visit_5 0.8" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
+    <sheet name="Impedance Spectroscopy S3" sheetId="4" r:id="rId1"/>
+    <sheet name="Impedance Spectroscopy 1 S2" sheetId="3" r:id="rId2"/>
+    <sheet name="Impedance Spectroscopy 2 S1" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,9 +39,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="14">
   <si>
-    <t>54_visit_5</t>
+    <t>Impedance Spectroscopy [2]</t>
   </si>
   <si>
     <t>TimeScan at 65 freqs [1]</t>
@@ -67,13 +68,19 @@
     <t>Cs / F</t>
   </si>
   <si>
-    <t>54_visit_3</t>
+    <t>Impedance Spectroscopy [1]</t>
   </si>
   <si>
     <t>TimeScan at 65 freqs</t>
   </si>
   <si>
     <t>22/11/2024 15:49:23</t>
+  </si>
+  <si>
+    <t>Impedance Spectroscopy</t>
+  </si>
+  <si>
+    <t>TimeScan at 60 freqs</t>
   </si>
 </sst>
 </file>
@@ -445,7 +452,2816 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C68FCC3D-176F-43E3-B71E-38E1F098604D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{873A4624-3CD1-4285-85ED-DFA08B90283F}">
+  <dimension ref="A1:G122"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="1">
+        <v>45515.584363425929</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3">
+        <v>80000</v>
+      </c>
+      <c r="B3">
+        <v>46.90226861249095</v>
+      </c>
+      <c r="C3">
+        <v>-0.31232833862304688</v>
+      </c>
+      <c r="D3">
+        <v>162.6685173870284</v>
+      </c>
+      <c r="E3">
+        <v>111.14242880282255</v>
+      </c>
+      <c r="F3">
+        <v>118.77881574044878</v>
+      </c>
+      <c r="G3">
+        <v>1.6749087589793268E-8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A4">
+        <v>71923.3125</v>
+      </c>
+      <c r="B4">
+        <v>48.421789106735837</v>
+      </c>
+      <c r="C4">
+        <v>-0.25510787963867188</v>
+      </c>
+      <c r="D4">
+        <v>171.88847929696362</v>
+      </c>
+      <c r="E4">
+        <v>114.07237692551401</v>
+      </c>
+      <c r="F4">
+        <v>128.58126666659555</v>
+      </c>
+      <c r="G4">
+        <v>1.7209678249133926E-8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A5">
+        <v>64662.03125</v>
+      </c>
+      <c r="B5">
+        <v>49.997370135917556</v>
+      </c>
+      <c r="C5">
+        <v>-0.23603439331054688</v>
+      </c>
+      <c r="D5">
+        <v>182.14571215618639</v>
+      </c>
+      <c r="E5">
+        <v>117.0874112840071</v>
+      </c>
+      <c r="F5">
+        <v>139.52633649492154</v>
+      </c>
+      <c r="G5">
+        <v>1.7640650563388281E-8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A6">
+        <v>58133.84375</v>
+      </c>
+      <c r="B6">
+        <v>51.532204827566268</v>
+      </c>
+      <c r="C6">
+        <v>-0.30279159545898438</v>
+      </c>
+      <c r="D6">
+        <v>193.4729590752801</v>
+      </c>
+      <c r="E6">
+        <v>120.35462324609576</v>
+      </c>
+      <c r="F6">
+        <v>151.48118878803189</v>
+      </c>
+      <c r="G6">
+        <v>1.8073089027916427E-8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A7">
+        <v>52264.73046875</v>
+      </c>
+      <c r="B7">
+        <v>53.037830543461119</v>
+      </c>
+      <c r="C7">
+        <v>-0.28371810913085938</v>
+      </c>
+      <c r="D7">
+        <v>205.72569768065253</v>
+      </c>
+      <c r="E7">
+        <v>123.70030667678118</v>
+      </c>
+      <c r="F7">
+        <v>164.38155861975983</v>
+      </c>
+      <c r="G7">
+        <v>1.8525004518792053E-8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A8">
+        <v>46988.15625</v>
+      </c>
+      <c r="B8">
+        <v>54.467931393415732</v>
+      </c>
+      <c r="C8">
+        <v>-0.25987625122070313</v>
+      </c>
+      <c r="D8">
+        <v>219.49652017574874</v>
+      </c>
+      <c r="E8">
+        <v>127.5622744438587</v>
+      </c>
+      <c r="F8">
+        <v>178.62415432402344</v>
+      </c>
+      <c r="G8">
+        <v>1.8962323075644977E-8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A9">
+        <v>42244.296875</v>
+      </c>
+      <c r="B9">
+        <v>55.963240708446705</v>
+      </c>
+      <c r="C9">
+        <v>-0.28848648071289063</v>
+      </c>
+      <c r="D9">
+        <v>234.43441188580792</v>
+      </c>
+      <c r="E9">
+        <v>131.21872489334385</v>
+      </c>
+      <c r="F9">
+        <v>194.27078965611267</v>
+      </c>
+      <c r="G9">
+        <v>1.9392979580702353E-8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A10">
+        <v>37979.37109375</v>
+      </c>
+      <c r="B10">
+        <v>57.335615551595417</v>
+      </c>
+      <c r="C10">
+        <v>-0.22172927856445313</v>
+      </c>
+      <c r="D10">
+        <v>251.11073901807268</v>
+      </c>
+      <c r="E10">
+        <v>135.52876631148894</v>
+      </c>
+      <c r="F10">
+        <v>211.39668103423105</v>
+      </c>
+      <c r="G10">
+        <v>1.9823219879903452E-8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A11">
+        <v>34145.02734375</v>
+      </c>
+      <c r="B11">
+        <v>58.757100896127618</v>
+      </c>
+      <c r="C11">
+        <v>-0.19788742065429688</v>
+      </c>
+      <c r="D11">
+        <v>269.13752415646928</v>
+      </c>
+      <c r="E11">
+        <v>139.59283339043898</v>
+      </c>
+      <c r="F11">
+        <v>230.10616631264628</v>
+      </c>
+      <c r="G11">
+        <v>2.0256500071756204E-8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A12">
+        <v>30697.791015625</v>
+      </c>
+      <c r="B12">
+        <v>60.096195833381799</v>
+      </c>
+      <c r="C12">
+        <v>-0.29802322387695313</v>
+      </c>
+      <c r="D12">
+        <v>289.32353606719289</v>
+      </c>
+      <c r="E12">
+        <v>144.24088806334996</v>
+      </c>
+      <c r="F12">
+        <v>250.80405645268263</v>
+      </c>
+      <c r="G12">
+        <v>2.0671807403120813E-8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A13">
+        <v>27598.583984375</v>
+      </c>
+      <c r="B13">
+        <v>61.38628429166684</v>
+      </c>
+      <c r="C13">
+        <v>-0.31709671020507813</v>
+      </c>
+      <c r="D13">
+        <v>311.23278167416169</v>
+      </c>
+      <c r="E13">
+        <v>149.05000768964584</v>
+      </c>
+      <c r="F13">
+        <v>273.2214113065682</v>
+      </c>
+      <c r="G13">
+        <v>2.1106615626855638E-8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A14">
+        <v>24812.26953125</v>
+      </c>
+      <c r="B14">
+        <v>62.634876540959155</v>
+      </c>
+      <c r="C14">
+        <v>-0.26464462280273438</v>
+      </c>
+      <c r="D14">
+        <v>335.94645043244623</v>
+      </c>
+      <c r="E14">
+        <v>154.42090252893561</v>
+      </c>
+      <c r="F14">
+        <v>298.35248016450112</v>
+      </c>
+      <c r="G14">
+        <v>2.1499283622484685E-8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A15">
+        <v>22307.2578125</v>
+      </c>
+      <c r="B15">
+        <v>63.877913917803845</v>
+      </c>
+      <c r="C15">
+        <v>-0.29325485229492188</v>
+      </c>
+      <c r="D15">
+        <v>362.78176102105112</v>
+      </c>
+      <c r="E15">
+        <v>159.72747801291993</v>
+      </c>
+      <c r="F15">
+        <v>325.72647865527796</v>
+      </c>
+      <c r="G15">
+        <v>2.1903871388626641E-8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A16">
+        <v>20055.1484375</v>
+      </c>
+      <c r="B16">
+        <v>65.017555507034132</v>
+      </c>
+      <c r="C16">
+        <v>-0.28371810913085938</v>
+      </c>
+      <c r="D16">
+        <v>392.2909227931213</v>
+      </c>
+      <c r="E16">
+        <v>165.68036328140886</v>
+      </c>
+      <c r="F16">
+        <v>355.58709949718235</v>
+      </c>
+      <c r="G16">
+        <v>2.2317639304391341E-8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A17">
+        <v>18030.408203125</v>
+      </c>
+      <c r="B17">
+        <v>66.086137136959508</v>
+      </c>
+      <c r="C17">
+        <v>-0.23126602172851563</v>
+      </c>
+      <c r="D17">
+        <v>425.11921204327524</v>
+      </c>
+      <c r="E17">
+        <v>172.32750606909897</v>
+      </c>
+      <c r="F17">
+        <v>388.62523734351049</v>
+      </c>
+      <c r="G17">
+        <v>2.2713474422378358E-8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A18">
+        <v>16210.08203125</v>
+      </c>
+      <c r="B18">
+        <v>67.132993353566889</v>
+      </c>
+      <c r="C18">
+        <v>-0.25510787963867188</v>
+      </c>
+      <c r="D18">
+        <v>461.94182769670374</v>
+      </c>
+      <c r="E18">
+        <v>179.50755827245021</v>
+      </c>
+      <c r="F18">
+        <v>425.63750856666053</v>
+      </c>
+      <c r="G18">
+        <v>2.306720772834865E-8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A19">
+        <v>14573.53515625</v>
+      </c>
+      <c r="B19">
+        <v>68.156747518402454</v>
+      </c>
+      <c r="C19">
+        <v>-0.22649765014648438</v>
+      </c>
+      <c r="D19">
+        <v>501.29932168700554</v>
+      </c>
+      <c r="E19">
+        <v>186.51775783542078</v>
+      </c>
+      <c r="F19">
+        <v>465.30864588560917</v>
+      </c>
+      <c r="G19">
+        <v>2.3470054412282714E-8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A20">
+        <v>13102.2109375</v>
+      </c>
+      <c r="B20">
+        <v>69.107554503611539</v>
+      </c>
+      <c r="C20">
+        <v>-0.25033950805664063</v>
+      </c>
+      <c r="D20">
+        <v>545.85119303268209</v>
+      </c>
+      <c r="E20">
+        <v>194.65862520179144</v>
+      </c>
+      <c r="F20">
+        <v>509.9622972041667</v>
+      </c>
+      <c r="G20">
+        <v>2.3819765180534973E-8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A21">
+        <v>11779.4296875</v>
+      </c>
+      <c r="B21">
+        <v>69.938485187995724</v>
+      </c>
+      <c r="C21">
+        <v>-0.24557113647460938</v>
+      </c>
+      <c r="D21">
+        <v>593.25990157482568</v>
+      </c>
+      <c r="E21">
+        <v>203.50525220354024</v>
+      </c>
+      <c r="F21">
+        <v>557.26378237074164</v>
+      </c>
+      <c r="G21">
+        <v>2.424571797244802E-8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A22">
+        <v>10590.1953125</v>
+      </c>
+      <c r="B22">
+        <v>70.727255077508318</v>
+      </c>
+      <c r="C22">
+        <v>-0.25033950805664063</v>
+      </c>
+      <c r="D22">
+        <v>647.11418050378199</v>
+      </c>
+      <c r="E22">
+        <v>213.58999945376542</v>
+      </c>
+      <c r="F22">
+        <v>610.84865125693932</v>
+      </c>
+      <c r="G22">
+        <v>2.4602687061978319E-8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A23">
+        <v>9521.0234375</v>
+      </c>
+      <c r="B23">
+        <v>71.728904902732125</v>
+      </c>
+      <c r="C23">
+        <v>7.152557373046875E-3</v>
+      </c>
+      <c r="D23">
+        <v>702.10041627542932</v>
+      </c>
+      <c r="E23">
+        <v>220.11791984440919</v>
+      </c>
+      <c r="F23">
+        <v>666.70315425795116</v>
+      </c>
+      <c r="G23">
+        <v>2.5072866458509356E-8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A24">
+        <v>8559.7939453125</v>
+      </c>
+      <c r="B24">
+        <v>72.461586900324448</v>
+      </c>
+      <c r="C24">
+        <v>7.152557373046875E-3</v>
+      </c>
+      <c r="D24">
+        <v>766.18811011692321</v>
+      </c>
+      <c r="E24">
+        <v>230.88706113459293</v>
+      </c>
+      <c r="F24">
+        <v>730.57195749985726</v>
+      </c>
+      <c r="G24">
+        <v>2.5450353750216522E-8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A25">
+        <v>7695.609375</v>
+      </c>
+      <c r="B25">
+        <v>73.015313352948638</v>
+      </c>
+      <c r="C25">
+        <v>-2.384185791015625E-3</v>
+      </c>
+      <c r="D25">
+        <v>838.72338943206273</v>
+      </c>
+      <c r="E25">
+        <v>245.00460903414245</v>
+      </c>
+      <c r="F25">
+        <v>802.14067689678632</v>
+      </c>
+      <c r="G25">
+        <v>2.5782592019761178E-8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A26">
+        <v>6918.6708984375</v>
+      </c>
+      <c r="B26">
+        <v>73.650657973692915</v>
+      </c>
+      <c r="C26">
+        <v>7.152557373046875E-3</v>
+      </c>
+      <c r="D26">
+        <v>915.62510109712855</v>
+      </c>
+      <c r="E26">
+        <v>257.7422128345255</v>
+      </c>
+      <c r="F26">
+        <v>878.60018067508338</v>
+      </c>
+      <c r="G26">
+        <v>2.6182202076937773E-8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A27">
+        <v>6220.171875</v>
+      </c>
+      <c r="B27">
+        <v>74.200518377980885</v>
+      </c>
+      <c r="C27">
+        <v>-7.152557373046875E-3</v>
+      </c>
+      <c r="D27">
+        <v>1003.1263367951493</v>
+      </c>
+      <c r="E27">
+        <v>273.12275399424118</v>
+      </c>
+      <c r="F27">
+        <v>965.22868213841252</v>
+      </c>
+      <c r="G27">
+        <v>2.6508644914328929E-8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A28">
+        <v>5592.19189453125</v>
+      </c>
+      <c r="B28">
+        <v>74.764162081003576</v>
+      </c>
+      <c r="C28">
+        <v>1.6689300537109375E-2</v>
+      </c>
+      <c r="D28">
+        <v>1097.5331137440071</v>
+      </c>
+      <c r="E28">
+        <v>288.42372890499689</v>
+      </c>
+      <c r="F28">
+        <v>1058.9573590891903</v>
+      </c>
+      <c r="G28">
+        <v>2.6875688152074719E-8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A29">
+        <v>5027.61181640625</v>
+      </c>
+      <c r="B29">
+        <v>75.218624721033962</v>
+      </c>
+      <c r="C29">
+        <v>-7.152557373046875E-3</v>
+      </c>
+      <c r="D29">
+        <v>1202.2122956588616</v>
+      </c>
+      <c r="E29">
+        <v>306.72218569928009</v>
+      </c>
+      <c r="F29">
+        <v>1162.4267308665981</v>
+      </c>
+      <c r="G29">
+        <v>2.723283188295968E-8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A30">
+        <v>4520.03125</v>
+      </c>
+      <c r="B30">
+        <v>75.602133273682071</v>
+      </c>
+      <c r="C30">
+        <v>-2.4080276489257813E-2</v>
+      </c>
+      <c r="D30">
+        <v>1318.3776785310467</v>
+      </c>
+      <c r="E30">
+        <v>327.81965134192177</v>
+      </c>
+      <c r="F30">
+        <v>1276.9706259123477</v>
+      </c>
+      <c r="G30">
+        <v>2.7573874012430482E-8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A31">
+        <v>4063.695068359375</v>
+      </c>
+      <c r="B31">
+        <v>76.019210099016007</v>
+      </c>
+      <c r="C31">
+        <v>-5.4836273193359375E-3</v>
+      </c>
+      <c r="D31">
+        <v>1445.5889007627618</v>
+      </c>
+      <c r="E31">
+        <v>349.24930814872965</v>
+      </c>
+      <c r="F31">
+        <v>1402.7659073295599</v>
+      </c>
+      <c r="G31">
+        <v>2.791989736408239E-8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A32">
+        <v>3653.429931640625</v>
+      </c>
+      <c r="B32">
+        <v>76.35141968190365</v>
+      </c>
+      <c r="C32">
+        <v>1.1205673217773438E-2</v>
+      </c>
+      <c r="D32">
+        <v>1582.6515156642797</v>
+      </c>
+      <c r="E32">
+        <v>373.45217084780677</v>
+      </c>
+      <c r="F32">
+        <v>1537.9594585435279</v>
+      </c>
+      <c r="G32">
+        <v>2.8325296313132304E-8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A33">
+        <v>3284.584716796875</v>
+      </c>
+      <c r="B33">
+        <v>76.783451731554536</v>
+      </c>
+      <c r="C33">
+        <v>-1.1682510375976563E-2</v>
+      </c>
+      <c r="D33">
+        <v>1739.5123312465425</v>
+      </c>
+      <c r="E33">
+        <v>397.70827266639492</v>
+      </c>
+      <c r="F33">
+        <v>1693.4377108153383</v>
+      </c>
+      <c r="G33">
+        <v>2.8613463974320127E-8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A34">
+        <v>2952.9775390625</v>
+      </c>
+      <c r="B34">
+        <v>77.035845982395529</v>
+      </c>
+      <c r="C34">
+        <v>-2.6464462280273438E-2</v>
+      </c>
+      <c r="D34">
+        <v>1903.3443581544982</v>
+      </c>
+      <c r="E34">
+        <v>426.99896617868865</v>
+      </c>
+      <c r="F34">
+        <v>1854.8292720897225</v>
+      </c>
+      <c r="G34">
+        <v>2.9057352830871009E-8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A35">
+        <v>2654.84912109375</v>
+      </c>
+      <c r="B35">
+        <v>77.294156666843719</v>
+      </c>
+      <c r="C35">
+        <v>-3.8385391235351563E-2</v>
+      </c>
+      <c r="D35">
+        <v>2091.7273347015416</v>
+      </c>
+      <c r="E35">
+        <v>460.06641922883637</v>
+      </c>
+      <c r="F35">
+        <v>2040.5053620697918</v>
+      </c>
+      <c r="G35">
+        <v>2.9379374602806245E-8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A36">
+        <v>2386.819091796875</v>
+      </c>
+      <c r="B36">
+        <v>77.520163959201597</v>
+      </c>
+      <c r="C36">
+        <v>-8.3446502685546875E-3</v>
+      </c>
+      <c r="D36">
+        <v>2292.3627575021519</v>
+      </c>
+      <c r="E36">
+        <v>495.37045717445187</v>
+      </c>
+      <c r="F36">
+        <v>2238.1990800957906</v>
+      </c>
+      <c r="G36">
+        <v>2.9792154785782495E-8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A37">
+        <v>2145.84912109375</v>
+      </c>
+      <c r="B37">
+        <v>77.812040814618754</v>
+      </c>
+      <c r="C37">
+        <v>-1.5497207641601563E-2</v>
+      </c>
+      <c r="D37">
+        <v>2516.9239807178051</v>
+      </c>
+      <c r="E37">
+        <v>531.37144547455944</v>
+      </c>
+      <c r="F37">
+        <v>2460.193226485806</v>
+      </c>
+      <c r="G37">
+        <v>3.0147529624999465E-8</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A38">
+        <v>1929.2071533203125</v>
+      </c>
+      <c r="B38">
+        <v>78.06909042485924</v>
+      </c>
+      <c r="C38">
+        <v>-1.0728836059570313E-2</v>
+      </c>
+      <c r="D38">
+        <v>2759.8081369236934</v>
+      </c>
+      <c r="E38">
+        <v>570.5407534070664</v>
+      </c>
+      <c r="F38">
+        <v>2700.189660252021</v>
+      </c>
+      <c r="G38">
+        <v>3.0552517263248546E-8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A39">
+        <v>1734.4371337890625</v>
+      </c>
+      <c r="B39">
+        <v>78.04188822099016</v>
+      </c>
+      <c r="C39">
+        <v>-5.9604644775390625E-3</v>
+      </c>
+      <c r="D39">
+        <v>3024.6647263971927</v>
+      </c>
+      <c r="E39">
+        <v>626.70001744591013</v>
+      </c>
+      <c r="F39">
+        <v>2959.0275083622828</v>
+      </c>
+      <c r="G39">
+        <v>3.1010771147069016E-8</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A40">
+        <v>1559.3306884765625</v>
+      </c>
+      <c r="B40">
+        <v>78.480193345627256</v>
+      </c>
+      <c r="C40">
+        <v>-2.4080276489257813E-2</v>
+      </c>
+      <c r="D40">
+        <v>3330.7241551762363</v>
+      </c>
+      <c r="E40">
+        <v>665.16784295831872</v>
+      </c>
+      <c r="F40">
+        <v>3263.6291361869889</v>
+      </c>
+      <c r="G40">
+        <v>3.1273832360872304E-8</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A41">
+        <v>1401.90283203125</v>
+      </c>
+      <c r="B41">
+        <v>78.464180788641045</v>
+      </c>
+      <c r="C41">
+        <v>-3.0279159545898438E-2</v>
+      </c>
+      <c r="D41">
+        <v>3660.3507519900354</v>
+      </c>
+      <c r="E41">
+        <v>731.99880377900104</v>
+      </c>
+      <c r="F41">
+        <v>3586.4112116236934</v>
+      </c>
+      <c r="G41">
+        <v>3.1654986674657087E-8</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A42">
+        <v>1260.36865234375</v>
+      </c>
+      <c r="B42">
+        <v>78.681380385983587</v>
+      </c>
+      <c r="C42">
+        <v>-3.3617019653320313E-2</v>
+      </c>
+      <c r="D42">
+        <v>3997.4276571456517</v>
+      </c>
+      <c r="E42">
+        <v>784.55437057067604</v>
+      </c>
+      <c r="F42">
+        <v>3919.6814046209706</v>
+      </c>
+      <c r="G42">
+        <v>3.2216011387086919E-8</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A43">
+        <v>1133.1236572265625</v>
+      </c>
+      <c r="B43">
+        <v>78.801182554239162</v>
+      </c>
+      <c r="C43">
+        <v>-8.3446502685546875E-3</v>
+      </c>
+      <c r="D43">
+        <v>4402.8517413552463</v>
+      </c>
+      <c r="E43">
+        <v>855.09590946578624</v>
+      </c>
+      <c r="F43">
+        <v>4319.0177635626605</v>
+      </c>
+      <c r="G43">
+        <v>3.2520546455284892E-8</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A44">
+        <v>1018.7250366210938</v>
+      </c>
+      <c r="B44">
+        <v>78.578786135255399</v>
+      </c>
+      <c r="C44">
+        <v>-1.1682510375976563E-2</v>
+      </c>
+      <c r="D44">
+        <v>4815.42269256905</v>
+      </c>
+      <c r="E44">
+        <v>953.55132089655399</v>
+      </c>
+      <c r="F44">
+        <v>4720.067328600875</v>
+      </c>
+      <c r="G44">
+        <v>3.3099006512368178E-8</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A45">
+        <v>915.8759765625</v>
+      </c>
+      <c r="B45">
+        <v>78.71244621971907</v>
+      </c>
+      <c r="C45">
+        <v>1.2159347534179688E-2</v>
+      </c>
+      <c r="D45">
+        <v>5310.6555048461669</v>
+      </c>
+      <c r="E45">
+        <v>1039.4711878685516</v>
+      </c>
+      <c r="F45">
+        <v>5207.9325591585803</v>
+      </c>
+      <c r="G45">
+        <v>3.3367073068749499E-8</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A46">
+        <v>823.410400390625</v>
+      </c>
+      <c r="B46">
+        <v>78.81492223045295</v>
+      </c>
+      <c r="C46">
+        <v>5.4836273193359375E-3</v>
+      </c>
+      <c r="D46">
+        <v>5840.7578827411899</v>
+      </c>
+      <c r="E46">
+        <v>1132.9835711706151</v>
+      </c>
+      <c r="F46">
+        <v>5729.8168271124359</v>
+      </c>
+      <c r="G46">
+        <v>3.3733627496449134E-8</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A47">
+        <v>740.280029296875</v>
+      </c>
+      <c r="B47">
+        <v>78.611108292128762</v>
+      </c>
+      <c r="C47">
+        <v>2.1457672119140625E-3</v>
+      </c>
+      <c r="D47">
+        <v>6422.139201176783</v>
+      </c>
+      <c r="E47">
+        <v>1268.1623941623998</v>
+      </c>
+      <c r="F47">
+        <v>6295.6839232385109</v>
+      </c>
+      <c r="G47">
+        <v>3.414925095827617E-8</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A48">
+        <v>665.5423583984375</v>
+      </c>
+      <c r="B48">
+        <v>78.661652697217619</v>
+      </c>
+      <c r="C48">
+        <v>7.3909759521484375E-3</v>
+      </c>
+      <c r="D48">
+        <v>7069.5929552901771</v>
+      </c>
+      <c r="E48">
+        <v>1389.8990314546268</v>
+      </c>
+      <c r="F48">
+        <v>6931.6177935493524</v>
+      </c>
+      <c r="G48">
+        <v>3.4499263395771279E-8</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A49">
+        <v>598.35009765625</v>
+      </c>
+      <c r="B49">
+        <v>78.646623409584791</v>
+      </c>
+      <c r="C49">
+        <v>5.0067901611328125E-3</v>
+      </c>
+      <c r="D49">
+        <v>7737.6757450153518</v>
+      </c>
+      <c r="E49">
+        <v>1523.235728862423</v>
+      </c>
+      <c r="F49">
+        <v>7586.2625085951149</v>
+      </c>
+      <c r="G49">
+        <v>3.5062017228665552E-8</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A50">
+        <v>537.9415283203125</v>
+      </c>
+      <c r="B50">
+        <v>78.646949900996319</v>
+      </c>
+      <c r="C50">
+        <v>3.5047531127929688E-2</v>
+      </c>
+      <c r="D50">
+        <v>8519.5867436202352</v>
+      </c>
+      <c r="E50">
+        <v>1677.114815314784</v>
+      </c>
+      <c r="F50">
+        <v>8352.8823874349691</v>
+      </c>
+      <c r="G50">
+        <v>3.5420011085332782E-8</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A51">
+        <v>483.63168334960938</v>
+      </c>
+      <c r="B51">
+        <v>78.650266180297933</v>
+      </c>
+      <c r="C51">
+        <v>3.6001205444335938E-2</v>
+      </c>
+      <c r="D51">
+        <v>9362.4378048888302</v>
+      </c>
+      <c r="E51">
+        <v>1842.5021291837722</v>
+      </c>
+      <c r="F51">
+        <v>9179.3478828490242</v>
+      </c>
+      <c r="G51">
+        <v>3.5850363051954771E-8</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A52">
+        <v>434.80490112304688</v>
+      </c>
+      <c r="B52">
+        <v>78.595007524973767</v>
+      </c>
+      <c r="C52">
+        <v>3.5524368286132813E-2</v>
+      </c>
+      <c r="D52">
+        <v>10290.867816873531</v>
+      </c>
+      <c r="E52">
+        <v>2034.944560467618</v>
+      </c>
+      <c r="F52">
+        <v>10087.663805866385</v>
+      </c>
+      <c r="G52">
+        <v>3.6285666182212666E-8</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A53">
+        <v>390.9075927734375</v>
+      </c>
+      <c r="B53">
+        <v>78.449696624975985</v>
+      </c>
+      <c r="C53">
+        <v>3.5524368286132813E-2</v>
+      </c>
+      <c r="D53">
+        <v>11297.996486740371</v>
+      </c>
+      <c r="E53">
+        <v>2262.1774062751997</v>
+      </c>
+      <c r="F53">
+        <v>11069.204036286248</v>
+      </c>
+      <c r="G53">
+        <v>3.6781516639192677E-8</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A54">
+        <v>351.44210815429688</v>
+      </c>
+      <c r="B54">
+        <v>78.345044392438055</v>
+      </c>
+      <c r="C54">
+        <v>3.3974647521972656E-2</v>
+      </c>
+      <c r="D54">
+        <v>12418.412480592528</v>
+      </c>
+      <c r="E54">
+        <v>2508.7353303549435</v>
+      </c>
+      <c r="F54">
+        <v>12162.368830962376</v>
+      </c>
+      <c r="G54">
+        <v>3.7234726375178455E-8</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A55">
+        <v>315.96099853515625</v>
+      </c>
+      <c r="B55">
+        <v>78.299217770135044</v>
+      </c>
+      <c r="C55">
+        <v>1.3113021850585938E-3</v>
+      </c>
+      <c r="D55">
+        <v>13628.046435276518</v>
+      </c>
+      <c r="E55">
+        <v>2763.7768683314143</v>
+      </c>
+      <c r="F55">
+        <v>13344.856202452283</v>
+      </c>
+      <c r="G55">
+        <v>3.7746158183079366E-8</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A56">
+        <v>284.06201171875</v>
+      </c>
+      <c r="B56">
+        <v>78.153656687904444</v>
+      </c>
+      <c r="C56">
+        <v>1.0251998901367188E-3</v>
+      </c>
+      <c r="D56">
+        <v>14960.424636820122</v>
+      </c>
+      <c r="E56">
+        <v>3071.1916923938907</v>
+      </c>
+      <c r="F56">
+        <v>14641.792475736884</v>
+      </c>
+      <c r="G56">
+        <v>3.8265969951177316E-8</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A57">
+        <v>255.38351440429688</v>
+      </c>
+      <c r="B57">
+        <v>77.941768547449328</v>
+      </c>
+      <c r="C57">
+        <v>2.7894973754882813E-3</v>
+      </c>
+      <c r="D57">
+        <v>16430.655585031709</v>
+      </c>
+      <c r="E57">
+        <v>3432.4576817262041</v>
+      </c>
+      <c r="F57">
+        <v>16068.126126499395</v>
+      </c>
+      <c r="G57">
+        <v>3.8784843240190928E-8</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A58">
+        <v>229.600341796875</v>
+      </c>
+      <c r="B58">
+        <v>77.791202612168746</v>
+      </c>
+      <c r="C58">
+        <v>4.9829483032226563E-3</v>
+      </c>
+      <c r="D58">
+        <v>18044.946988092965</v>
+      </c>
+      <c r="E58">
+        <v>3816.0528131763117</v>
+      </c>
+      <c r="F58">
+        <v>17636.83227595405</v>
+      </c>
+      <c r="G58">
+        <v>3.9303119023373324E-8</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A59">
+        <v>206.42021179199219</v>
+      </c>
+      <c r="B59">
+        <v>77.606773436339807</v>
+      </c>
+      <c r="C59">
+        <v>6.8902969360351563E-3</v>
+      </c>
+      <c r="D59">
+        <v>19781.29777761886</v>
+      </c>
+      <c r="E59">
+        <v>4245.4594521374765</v>
+      </c>
+      <c r="F59">
+        <v>19320.347196856619</v>
+      </c>
+      <c r="G59">
+        <v>3.9907358798013168E-8</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A60">
+        <v>185.58030700683594</v>
+      </c>
+      <c r="B60">
+        <v>77.345567168018079</v>
+      </c>
+      <c r="C60">
+        <v>6.8426132202148438E-3</v>
+      </c>
+      <c r="D60">
+        <v>21729.73761513321</v>
+      </c>
+      <c r="E60">
+        <v>4760.3400318444474</v>
+      </c>
+      <c r="F60">
+        <v>21201.902263800632</v>
+      </c>
+      <c r="G60">
+        <v>4.0449523936224635E-8</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A61">
+        <v>166.84437561035156</v>
+      </c>
+      <c r="B61">
+        <v>77.16784955480297</v>
+      </c>
+      <c r="C61">
+        <v>6.1273574829101563E-3</v>
+      </c>
+      <c r="D61">
+        <v>23770.800997464805</v>
+      </c>
+      <c r="E61">
+        <v>5279.3914834670331</v>
+      </c>
+      <c r="F61">
+        <v>23177.122462147228</v>
+      </c>
+      <c r="G61">
+        <v>4.1157505525718293E-8</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A62">
+        <v>150</v>
+      </c>
+      <c r="B62">
+        <v>76.879019429893077</v>
+      </c>
+      <c r="C62">
+        <v>4.7445297241210938E-3</v>
+      </c>
+      <c r="D62">
+        <v>26099.295378139701</v>
+      </c>
+      <c r="E62">
+        <v>5924.7473517884782</v>
+      </c>
+      <c r="F62">
+        <v>25417.918641243225</v>
+      </c>
+      <c r="G62">
+        <v>4.1743502641649513E-8</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A63">
+        <v>80000</v>
+      </c>
+      <c r="B63">
+        <v>44.964397595764133</v>
+      </c>
+      <c r="C63">
+        <v>-0.32186508178710938</v>
+      </c>
+      <c r="D63">
+        <v>148.53404820930268</v>
+      </c>
+      <c r="E63">
+        <v>105.09467554743682</v>
+      </c>
+      <c r="F63">
+        <v>104.96414935120676</v>
+      </c>
+      <c r="G63">
+        <v>1.8953488414335627E-8</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A64">
+        <v>71923.3125</v>
+      </c>
+      <c r="B64">
+        <v>46.748220883980707</v>
+      </c>
+      <c r="C64">
+        <v>-0.27894973754882813</v>
+      </c>
+      <c r="D64">
+        <v>157.14650151830864</v>
+      </c>
+      <c r="E64">
+        <v>107.67766395416335</v>
+      </c>
+      <c r="F64">
+        <v>114.45760623400285</v>
+      </c>
+      <c r="G64">
+        <v>1.9333291172228025E-8</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A65">
+        <v>64662.03125</v>
+      </c>
+      <c r="B65">
+        <v>48.480631830009692</v>
+      </c>
+      <c r="C65">
+        <v>-0.23603439331054688</v>
+      </c>
+      <c r="D65">
+        <v>166.6646251295092</v>
+      </c>
+      <c r="E65">
+        <v>110.47751106943534</v>
+      </c>
+      <c r="F65">
+        <v>124.78708594026317</v>
+      </c>
+      <c r="G65">
+        <v>1.9724279383163948E-8</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A66">
+        <v>58133.84375</v>
+      </c>
+      <c r="B66">
+        <v>50.132870128539814</v>
+      </c>
+      <c r="C66">
+        <v>-0.32663345336914063</v>
+      </c>
+      <c r="D66">
+        <v>176.95832638574763</v>
+      </c>
+      <c r="E66">
+        <v>113.43195231137663</v>
+      </c>
+      <c r="F66">
+        <v>135.82135867408471</v>
+      </c>
+      <c r="G66">
+        <v>2.0156866620589088E-8</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A67">
+        <v>52264.73046875</v>
+      </c>
+      <c r="B67">
+        <v>51.819035569563354</v>
+      </c>
+      <c r="C67">
+        <v>-0.27418136596679688</v>
+      </c>
+      <c r="D67">
+        <v>188.58499471952402</v>
+      </c>
+      <c r="E67">
+        <v>116.57330028126977</v>
+      </c>
+      <c r="F67">
+        <v>148.23955577002991</v>
+      </c>
+      <c r="G67">
+        <v>2.0542216956999164E-8</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A68">
+        <v>46988.15625</v>
+      </c>
+      <c r="B68">
+        <v>53.463657282160895</v>
+      </c>
+      <c r="C68">
+        <v>-0.25987625122070313</v>
+      </c>
+      <c r="D68">
+        <v>201.28041619752702</v>
+      </c>
+      <c r="E68">
+        <v>119.82878415106229</v>
+      </c>
+      <c r="F68">
+        <v>161.72466859922088</v>
+      </c>
+      <c r="G68">
+        <v>2.0943798820202478E-8</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A69">
+        <v>42244.296875</v>
+      </c>
+      <c r="B69">
+        <v>55.035468274641069</v>
+      </c>
+      <c r="C69">
+        <v>-0.30755996704101563</v>
+      </c>
+      <c r="D69">
+        <v>215.39441971686847</v>
+      </c>
+      <c r="E69">
+        <v>123.4359164287832</v>
+      </c>
+      <c r="F69">
+        <v>176.51722460018723</v>
+      </c>
+      <c r="G69">
+        <v>2.1343466426357569E-8</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A70">
+        <v>37979.37109375</v>
+      </c>
+      <c r="B70">
+        <v>56.590961021150058</v>
+      </c>
+      <c r="C70">
+        <v>-0.22172927856445313</v>
+      </c>
+      <c r="D70">
+        <v>230.75638621435147</v>
+      </c>
+      <c r="E70">
+        <v>127.05733657861833</v>
+      </c>
+      <c r="F70">
+        <v>192.62643380453949</v>
+      </c>
+      <c r="G70">
+        <v>2.1754869294188336E-8</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A71">
+        <v>34145.02734375</v>
+      </c>
+      <c r="B71">
+        <v>58.07175607816648</v>
+      </c>
+      <c r="C71">
+        <v>-0.17404556274414063</v>
+      </c>
+      <c r="D71">
+        <v>247.85681379982583</v>
+      </c>
+      <c r="E71">
+        <v>131.08075411975889</v>
+      </c>
+      <c r="F71">
+        <v>210.35882688015931</v>
+      </c>
+      <c r="G71">
+        <v>2.2158069825513448E-8</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A72">
+        <v>30697.791015625</v>
+      </c>
+      <c r="B72">
+        <v>59.530921740080906</v>
+      </c>
+      <c r="C72">
+        <v>-0.28371810913085938</v>
+      </c>
+      <c r="D72">
+        <v>266.61210485720511</v>
+      </c>
+      <c r="E72">
+        <v>135.19187442417572</v>
+      </c>
+      <c r="F72">
+        <v>229.79375871869809</v>
+      </c>
+      <c r="G72">
+        <v>2.2561853637017127E-8</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A73">
+        <v>27598.583984375</v>
+      </c>
+      <c r="B73">
+        <v>60.922107416346449</v>
+      </c>
+      <c r="C73">
+        <v>-0.32663345336914063</v>
+      </c>
+      <c r="D73">
+        <v>287.69920149879363</v>
+      </c>
+      <c r="E73">
+        <v>139.82129454743747</v>
+      </c>
+      <c r="F73">
+        <v>251.43753923016783</v>
+      </c>
+      <c r="G73">
+        <v>2.2935236031704121E-8</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A74">
+        <v>24812.26953125</v>
+      </c>
+      <c r="B74">
+        <v>62.293614732333829</v>
+      </c>
+      <c r="C74">
+        <v>-0.25510787963867188</v>
+      </c>
+      <c r="D74">
+        <v>310.84353902924533</v>
+      </c>
+      <c r="E74">
+        <v>144.52381716374501</v>
+      </c>
+      <c r="F74">
+        <v>275.20278346820254</v>
+      </c>
+      <c r="G74">
+        <v>2.330777512382782E-8</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A75">
+        <v>22307.2578125</v>
+      </c>
+      <c r="B75">
+        <v>63.609655397646897</v>
+      </c>
+      <c r="C75">
+        <v>-0.29802322387695313</v>
+      </c>
+      <c r="D75">
+        <v>336.42675299110203</v>
+      </c>
+      <c r="E75">
+        <v>149.53638588062114</v>
+      </c>
+      <c r="F75">
+        <v>301.36660303672994</v>
+      </c>
+      <c r="G75">
+        <v>2.3674391337469768E-8</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A76">
+        <v>20055.1484375</v>
+      </c>
+      <c r="B76">
+        <v>64.800389966813185</v>
+      </c>
+      <c r="C76">
+        <v>-0.27418136596679688</v>
+      </c>
+      <c r="D76">
+        <v>364.91053062270703</v>
+      </c>
+      <c r="E76">
+        <v>155.3690999305897</v>
+      </c>
+      <c r="F76">
+        <v>330.18197731872647</v>
+      </c>
+      <c r="G76">
+        <v>2.4034820714070346E-8</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A77">
+        <v>18030.408203125</v>
+      </c>
+      <c r="B77">
+        <v>65.981868723920286</v>
+      </c>
+      <c r="C77">
+        <v>-0.21696090698242188</v>
+      </c>
+      <c r="D77">
+        <v>395.95544899564811</v>
+      </c>
+      <c r="E77">
+        <v>161.16404957346489</v>
+      </c>
+      <c r="F77">
+        <v>361.67231953029949</v>
+      </c>
+      <c r="G77">
+        <v>2.4406151401788575E-8</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A78">
+        <v>16210.08203125</v>
+      </c>
+      <c r="B78">
+        <v>67.010053471613119</v>
+      </c>
+      <c r="C78">
+        <v>-0.23126602172851563</v>
+      </c>
+      <c r="D78">
+        <v>430.42593261035717</v>
+      </c>
+      <c r="E78">
+        <v>168.11128648309423</v>
+      </c>
+      <c r="F78">
+        <v>396.23866396465496</v>
+      </c>
+      <c r="G78">
+        <v>2.477867436974737E-8</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A79">
+        <v>14573.53515625</v>
+      </c>
+      <c r="B79">
+        <v>68.110578133217956</v>
+      </c>
+      <c r="C79">
+        <v>-0.21696090698242188</v>
+      </c>
+      <c r="D79">
+        <v>468.40755010012344</v>
+      </c>
+      <c r="E79">
+        <v>174.63005219394574</v>
+      </c>
+      <c r="F79">
+        <v>434.6377547585339</v>
+      </c>
+      <c r="G79">
+        <v>2.5126255411263055E-8</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A80">
+        <v>13102.2109375</v>
+      </c>
+      <c r="B80">
+        <v>69.050370625974693</v>
+      </c>
+      <c r="C80">
+        <v>-0.23603439331054688</v>
+      </c>
+      <c r="D80">
+        <v>510.55838127596218</v>
+      </c>
+      <c r="E80">
+        <v>182.54865306014113</v>
+      </c>
+      <c r="F80">
+        <v>476.80798017342261</v>
+      </c>
+      <c r="G80">
+        <v>2.5476046281589738E-8</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A81">
+        <v>11779.4296875</v>
+      </c>
+      <c r="B81">
+        <v>70.010558560450193</v>
+      </c>
+      <c r="C81">
+        <v>-0.24080276489257813</v>
+      </c>
+      <c r="D81">
+        <v>556.94132368050111</v>
+      </c>
+      <c r="E81">
+        <v>190.38870364386321</v>
+      </c>
+      <c r="F81">
+        <v>523.38874610350376</v>
+      </c>
+      <c r="G81">
+        <v>2.5814961831351086E-8</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A82">
+        <v>10590.1953125</v>
+      </c>
+      <c r="B82">
+        <v>70.810911664968089</v>
+      </c>
+      <c r="C82">
+        <v>-0.24080276489257813</v>
+      </c>
+      <c r="D82">
+        <v>608.85884678172999</v>
+      </c>
+      <c r="E82">
+        <v>200.12385961255382</v>
+      </c>
+      <c r="F82">
+        <v>575.03003062288235</v>
+      </c>
+      <c r="G82">
+        <v>2.6135188440205219E-8</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A83">
+        <v>9521.0234375</v>
+      </c>
+      <c r="B83">
+        <v>71.921416924273331</v>
+      </c>
+      <c r="C83">
+        <v>7.152557373046875E-3</v>
+      </c>
+      <c r="D83">
+        <v>660.3656788804509</v>
+      </c>
+      <c r="E83">
+        <v>204.92540988458549</v>
+      </c>
+      <c r="F83">
+        <v>627.76461052441744</v>
+      </c>
+      <c r="G83">
+        <v>2.6628068664482935E-8</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A84">
+        <v>8559.7939453125</v>
+      </c>
+      <c r="B84">
+        <v>72.657653406167256</v>
+      </c>
+      <c r="C84">
+        <v>2.384185791015625E-3</v>
+      </c>
+      <c r="D84">
+        <v>722.73171786509874</v>
+      </c>
+      <c r="E84">
+        <v>215.43219175541185</v>
+      </c>
+      <c r="F84">
+        <v>689.87687797439344</v>
+      </c>
+      <c r="G84">
+        <v>2.6951642172662664E-8</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A85">
+        <v>7695.609375</v>
+      </c>
+      <c r="B85">
+        <v>73.267078957938594</v>
+      </c>
+      <c r="C85">
+        <v>2.384185791015625E-3</v>
+      </c>
+      <c r="D85">
+        <v>791.8279172778665</v>
+      </c>
+      <c r="E85">
+        <v>227.97582384297635</v>
+      </c>
+      <c r="F85">
+        <v>758.29972591563023</v>
+      </c>
+      <c r="G85">
+        <v>2.7273207556435208E-8</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A86">
+        <v>6918.6708984375</v>
+      </c>
+      <c r="B86">
+        <v>73.924650276975811</v>
+      </c>
+      <c r="C86">
+        <v>2.384185791015625E-3</v>
+      </c>
+      <c r="D86">
+        <v>866.37761878556989</v>
+      </c>
+      <c r="E86">
+        <v>239.90106561047915</v>
+      </c>
+      <c r="F86">
+        <v>832.50084507555357</v>
+      </c>
+      <c r="G86">
+        <v>2.7632028977918183E-8</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A87">
+        <v>6220.171875</v>
+      </c>
+      <c r="B87">
+        <v>74.529671662647814</v>
+      </c>
+      <c r="C87">
+        <v>7.152557373046875E-3</v>
+      </c>
+      <c r="D87">
+        <v>951.3381476075192</v>
+      </c>
+      <c r="E87">
+        <v>253.75927792042455</v>
+      </c>
+      <c r="F87">
+        <v>916.86994713678484</v>
+      </c>
+      <c r="G87">
+        <v>2.7906797987910945E-8</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A88">
+        <v>5592.19189453125</v>
+      </c>
+      <c r="B88">
+        <v>75.020648822514033</v>
+      </c>
+      <c r="C88">
+        <v>2.1457672119140625E-2</v>
+      </c>
+      <c r="D88">
+        <v>1042.0714251695019</v>
+      </c>
+      <c r="E88">
+        <v>269.34515825204653</v>
+      </c>
+      <c r="F88">
+        <v>1006.6608370652833</v>
+      </c>
+      <c r="G88">
+        <v>2.8271893274596516E-8</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A89">
+        <v>5027.61181640625</v>
+      </c>
+      <c r="B89">
+        <v>75.541068993216712</v>
+      </c>
+      <c r="C89">
+        <v>-7.152557373046875E-3</v>
+      </c>
+      <c r="D89">
+        <v>1143.9632748011313</v>
+      </c>
+      <c r="E89">
+        <v>285.63159371689824</v>
+      </c>
+      <c r="F89">
+        <v>1107.730367356819</v>
+      </c>
+      <c r="G89">
+        <v>2.8577506468008098E-8</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A90">
+        <v>4520.03125</v>
+      </c>
+      <c r="B90">
+        <v>75.993786502239601</v>
+      </c>
+      <c r="C90">
+        <v>-9.7751617431640625E-3</v>
+      </c>
+      <c r="D90">
+        <v>1255.0427337644937</v>
+      </c>
+      <c r="E90">
+        <v>303.75437690094418</v>
+      </c>
+      <c r="F90">
+        <v>1217.7296670807414</v>
+      </c>
+      <c r="G90">
+        <v>2.8915306991651795E-8</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A91">
+        <v>4063.695068359375</v>
+      </c>
+      <c r="B91">
+        <v>76.40509296048846</v>
+      </c>
+      <c r="C91">
+        <v>-3.5762786865234375E-3</v>
+      </c>
+      <c r="D91">
+        <v>1375.7569093206339</v>
+      </c>
+      <c r="E91">
+        <v>323.37952481363385</v>
+      </c>
+      <c r="F91">
+        <v>1337.2108122785919</v>
+      </c>
+      <c r="G91">
+        <v>2.9288635568043586E-8</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A92">
+        <v>3653.429931640625</v>
+      </c>
+      <c r="B92">
+        <v>76.882579876535615</v>
+      </c>
+      <c r="C92">
+        <v>1.5020370483398438E-2</v>
+      </c>
+      <c r="D92">
+        <v>1510.9863123916093</v>
+      </c>
+      <c r="E92">
+        <v>342.9144500257139</v>
+      </c>
+      <c r="F92">
+        <v>1471.5601639750773</v>
+      </c>
+      <c r="G92">
+        <v>2.9603381803401241E-8</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A93">
+        <v>3284.584716796875</v>
+      </c>
+      <c r="B93">
+        <v>77.175850110356222</v>
+      </c>
+      <c r="C93">
+        <v>-3.0279159545898438E-2</v>
+      </c>
+      <c r="D93">
+        <v>1661.4381029699266</v>
+      </c>
+      <c r="E93">
+        <v>368.77196827440667</v>
+      </c>
+      <c r="F93">
+        <v>1619.9950016636867</v>
+      </c>
+      <c r="G93">
+        <v>2.9910659527595987E-8</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A94">
+        <v>2952.9775390625</v>
+      </c>
+      <c r="B94">
+        <v>77.349447271239768</v>
+      </c>
+      <c r="C94">
+        <v>-1.9311904907226563E-2</v>
+      </c>
+      <c r="D94">
+        <v>1825.2941887144611</v>
+      </c>
+      <c r="E94">
+        <v>399.74712827890227</v>
+      </c>
+      <c r="F94">
+        <v>1780.9831859923759</v>
+      </c>
+      <c r="G94">
+        <v>3.0262177107588613E-8</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A95">
+        <v>2654.84912109375</v>
+      </c>
+      <c r="B95">
+        <v>77.65412578272776</v>
+      </c>
+      <c r="C95">
+        <v>-1.5974044799804688E-2</v>
+      </c>
+      <c r="D95">
+        <v>2003.1469412600707</v>
+      </c>
+      <c r="E95">
+        <v>428.29804656126498</v>
+      </c>
+      <c r="F95">
+        <v>1956.8235616915954</v>
+      </c>
+      <c r="G95">
+        <v>3.0635757144839314E-8</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A96">
+        <v>2386.819091796875</v>
+      </c>
+      <c r="B96">
+        <v>77.882512427869955</v>
+      </c>
+      <c r="C96">
+        <v>-1.9311904907226563E-2</v>
+      </c>
+      <c r="D96">
+        <v>2201.8509813619721</v>
+      </c>
+      <c r="E96">
+        <v>462.20592590497313</v>
+      </c>
+      <c r="F96">
+        <v>2152.7920071811409</v>
+      </c>
+      <c r="G96">
+        <v>3.0974090025037479E-8</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A97">
+        <v>2145.84912109375</v>
+      </c>
+      <c r="B97">
+        <v>78.177815399901931</v>
+      </c>
+      <c r="C97">
+        <v>-1.6927719116210938E-2</v>
+      </c>
+      <c r="D97">
+        <v>2415.393980100956</v>
+      </c>
+      <c r="E97">
+        <v>494.85395855741143</v>
+      </c>
+      <c r="F97">
+        <v>2364.1589707141093</v>
+      </c>
+      <c r="G97">
+        <v>3.1372149291763029E-8</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A98">
+        <v>1929.2071533203125</v>
+      </c>
+      <c r="B98">
+        <v>78.404706820474985</v>
+      </c>
+      <c r="C98">
+        <v>-1.3113021850585938E-2</v>
+      </c>
+      <c r="D98">
+        <v>2668.0146388969765</v>
+      </c>
+      <c r="E98">
+        <v>536.26413587621039</v>
+      </c>
+      <c r="F98">
+        <v>2613.5651684894915</v>
+      </c>
+      <c r="G98">
+        <v>3.1565155598004293E-8</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A99">
+        <v>1734.4371337890625</v>
+      </c>
+      <c r="B99">
+        <v>78.734355448725367</v>
+      </c>
+      <c r="C99">
+        <v>-2.3603439331054688E-2</v>
+      </c>
+      <c r="D99">
+        <v>2927.2206425304603</v>
+      </c>
+      <c r="E99">
+        <v>571.85631309428356</v>
+      </c>
+      <c r="F99">
+        <v>2870.8188809520279</v>
+      </c>
+      <c r="G99">
+        <v>3.1963606442937405E-8</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A100">
+        <v>1559.3306884765625</v>
+      </c>
+      <c r="B100">
+        <v>78.934339997144249</v>
+      </c>
+      <c r="C100">
+        <v>-4.0531158447265625E-3</v>
+      </c>
+      <c r="D100">
+        <v>3201.8112595744497</v>
+      </c>
+      <c r="E100">
+        <v>614.53579596047234</v>
+      </c>
+      <c r="F100">
+        <v>3142.2827844452436</v>
+      </c>
+      <c r="G100">
+        <v>3.2481542080939648E-8</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A101">
+        <v>1401.90283203125</v>
+      </c>
+      <c r="B101">
+        <v>78.975536457010989</v>
+      </c>
+      <c r="C101">
+        <v>-1.7404556274414063E-2</v>
+      </c>
+      <c r="D101">
+        <v>3533.3852622381792</v>
+      </c>
+      <c r="E101">
+        <v>675.68255985265364</v>
+      </c>
+      <c r="F101">
+        <v>3468.1788433863862</v>
+      </c>
+      <c r="G101">
+        <v>3.2734124807398456E-8</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A102">
+        <v>1260.36865234375</v>
+      </c>
+      <c r="B102">
+        <v>79.242971900261125</v>
+      </c>
+      <c r="C102">
+        <v>-6.4373016357421875E-3</v>
+      </c>
+      <c r="D102">
+        <v>3901.238480890901</v>
+      </c>
+      <c r="E102">
+        <v>728.14488272574897</v>
+      </c>
+      <c r="F102">
+        <v>3832.6840092217685</v>
+      </c>
+      <c r="G102">
+        <v>3.2947276754668497E-8</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A103">
+        <v>1133.1236572265625</v>
+      </c>
+      <c r="B103">
+        <v>78.941090252705663</v>
+      </c>
+      <c r="C103">
+        <v>-1.6450881958007813E-2</v>
+      </c>
+      <c r="D103">
+        <v>4272.1157335787711</v>
+      </c>
+      <c r="E103">
+        <v>819.46943500510679</v>
+      </c>
+      <c r="F103">
+        <v>4192.7845981142045</v>
+      </c>
+      <c r="G103">
+        <v>3.3499650300259558E-8</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A104">
+        <v>1018.7250366210938</v>
+      </c>
+      <c r="B104">
+        <v>79.130363409697651</v>
+      </c>
+      <c r="C104">
+        <v>1.1682510375976563E-2</v>
+      </c>
+      <c r="D104">
+        <v>4693.709382729372</v>
+      </c>
+      <c r="E104">
+        <v>885.11641496110246</v>
+      </c>
+      <c r="F104">
+        <v>4609.498530370538</v>
+      </c>
+      <c r="G104">
+        <v>3.3892957817174534E-8</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A105">
+        <v>915.8759765625</v>
+      </c>
+      <c r="B105">
+        <v>79.038477258305022</v>
+      </c>
+      <c r="C105">
+        <v>1.6689300537109375E-3</v>
+      </c>
+      <c r="D105">
+        <v>5170.4591705923604</v>
+      </c>
+      <c r="E105">
+        <v>983.16144581853939</v>
+      </c>
+      <c r="F105">
+        <v>5076.1246641723292</v>
+      </c>
+      <c r="G105">
+        <v>3.4233490651849064E-8</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A106">
+        <v>823.410400390625</v>
+      </c>
+      <c r="B106">
+        <v>79.192176061892482</v>
+      </c>
+      <c r="C106">
+        <v>7.8678131103515625E-3</v>
+      </c>
+      <c r="D106">
+        <v>5692.0474566180892</v>
+      </c>
+      <c r="E106">
+        <v>1067.346826480938</v>
+      </c>
+      <c r="F106">
+        <v>5591.0799493830818</v>
+      </c>
+      <c r="G106">
+        <v>3.4570692642308631E-8</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A107">
+        <v>740.280029296875</v>
+      </c>
+      <c r="B107">
+        <v>79.251987073103621</v>
+      </c>
+      <c r="C107">
+        <v>1.6689300537109375E-3</v>
+      </c>
+      <c r="D107">
+        <v>6255.312258627534</v>
+      </c>
+      <c r="E107">
+        <v>1166.5529552030889</v>
+      </c>
+      <c r="F107">
+        <v>6145.5744772675926</v>
+      </c>
+      <c r="G107">
+        <v>3.4983367469373736E-8</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A108">
+        <v>665.5423583984375</v>
+      </c>
+      <c r="B108">
+        <v>78.973687537201513</v>
+      </c>
+      <c r="C108">
+        <v>3.0994415283203125E-3</v>
+      </c>
+      <c r="D108">
+        <v>6879.4751541214973</v>
+      </c>
+      <c r="E108">
+        <v>1315.7668827127061</v>
+      </c>
+      <c r="F108">
+        <v>6752.4762795978404</v>
+      </c>
+      <c r="G108">
+        <v>3.5414520261404951E-8</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A109">
+        <v>598.35009765625</v>
+      </c>
+      <c r="B109">
+        <v>78.913319348703382</v>
+      </c>
+      <c r="C109">
+        <v>1.0728836059570313E-2</v>
+      </c>
+      <c r="D109">
+        <v>7583.2289255179667</v>
+      </c>
+      <c r="E109">
+        <v>1458.2082374838642</v>
+      </c>
+      <c r="F109">
+        <v>7441.7060996082464</v>
+      </c>
+      <c r="G109">
+        <v>3.5743102887595089E-8</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A110">
+        <v>537.9415283203125</v>
+      </c>
+      <c r="B110">
+        <v>78.934657172734589</v>
+      </c>
+      <c r="C110">
+        <v>3.6478042602539063E-2</v>
+      </c>
+      <c r="D110">
+        <v>8335.8419260553728</v>
+      </c>
+      <c r="E110">
+        <v>1599.8845142243397</v>
+      </c>
+      <c r="F110">
+        <v>8180.8697677769997</v>
+      </c>
+      <c r="G110">
+        <v>3.6164759390592501E-8</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A111">
+        <v>483.63168334960938</v>
+      </c>
+      <c r="B111">
+        <v>78.83390006440348</v>
+      </c>
+      <c r="C111">
+        <v>3.6954879760742188E-2</v>
+      </c>
+      <c r="D111">
+        <v>9163.1994701068688</v>
+      </c>
+      <c r="E111">
+        <v>1774.4894763797097</v>
+      </c>
+      <c r="F111">
+        <v>8989.7392413342259</v>
+      </c>
+      <c r="G111">
+        <v>3.6606507190690062E-8</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A112">
+        <v>434.80490112304688</v>
+      </c>
+      <c r="B112">
+        <v>78.78715647924102</v>
+      </c>
+      <c r="C112">
+        <v>3.6478042602539063E-2</v>
+      </c>
+      <c r="D112">
+        <v>10075.030115910826</v>
+      </c>
+      <c r="E112">
+        <v>1959.1323134639208</v>
+      </c>
+      <c r="F112">
+        <v>9882.7138183219504</v>
+      </c>
+      <c r="G112">
+        <v>3.7038166656151185E-8</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A113">
+        <v>390.9075927734375</v>
+      </c>
+      <c r="B113">
+        <v>78.694627064503536</v>
+      </c>
+      <c r="C113">
+        <v>3.6478042602539063E-2</v>
+      </c>
+      <c r="D113">
+        <v>11063.182248513298</v>
+      </c>
+      <c r="E113">
+        <v>2168.8052382111323</v>
+      </c>
+      <c r="F113">
+        <v>10848.515350154034</v>
+      </c>
+      <c r="G113">
+        <v>3.7529754007998943E-8</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A114">
+        <v>351.44210815429688</v>
+      </c>
+      <c r="B114">
+        <v>78.523306823558684</v>
+      </c>
+      <c r="C114">
+        <v>3.7431716918945313E-2</v>
+      </c>
+      <c r="D114">
+        <v>12188.641822973939</v>
+      </c>
+      <c r="E114">
+        <v>2425.1655725319029</v>
+      </c>
+      <c r="F114">
+        <v>11944.938737162091</v>
+      </c>
+      <c r="G114">
+        <v>3.7912498796329147E-8</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A115">
+        <v>315.96099853515625</v>
+      </c>
+      <c r="B115">
+        <v>78.383667296696174</v>
+      </c>
+      <c r="C115">
+        <v>2.0265579223632813E-3</v>
+      </c>
+      <c r="D115">
+        <v>13374.267918364403</v>
+      </c>
+      <c r="E115">
+        <v>2693.0044734221283</v>
+      </c>
+      <c r="F115">
+        <v>13100.334700240284</v>
+      </c>
+      <c r="G115">
+        <v>3.8450701044987242E-8</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A116">
+        <v>284.06201171875</v>
+      </c>
+      <c r="B116">
+        <v>78.212955476411935</v>
+      </c>
+      <c r="C116">
+        <v>2.0742416381835938E-3</v>
+      </c>
+      <c r="D116">
+        <v>14693.436723360199</v>
+      </c>
+      <c r="E116">
+        <v>3001.4975154579415</v>
+      </c>
+      <c r="F116">
+        <v>14383.605090800076</v>
+      </c>
+      <c r="G116">
+        <v>3.8952848564111723E-8</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A117">
+        <v>255.38351440429688</v>
+      </c>
+      <c r="B117">
+        <v>77.96547090539147</v>
+      </c>
+      <c r="C117">
+        <v>3.7431716918945313E-3</v>
+      </c>
+      <c r="D117">
+        <v>16150.260716461309</v>
+      </c>
+      <c r="E117">
+        <v>3367.3476115390581</v>
+      </c>
+      <c r="F117">
+        <v>15795.312319569231</v>
+      </c>
+      <c r="G117">
+        <v>3.9454728109921362E-8</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A118">
+        <v>229.600341796875</v>
+      </c>
+      <c r="B118">
+        <v>77.820406431036716</v>
+      </c>
+      <c r="C118">
+        <v>5.6982040405273438E-3</v>
+      </c>
+      <c r="D118">
+        <v>17744.659993899051</v>
+      </c>
+      <c r="E118">
+        <v>3743.7092259524557</v>
+      </c>
+      <c r="F118">
+        <v>17345.247174099306</v>
+      </c>
+      <c r="G118">
+        <v>3.9963830505234035E-8</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A119">
+        <v>206.42021179199219</v>
+      </c>
+      <c r="B119">
+        <v>77.547026390203229</v>
+      </c>
+      <c r="C119">
+        <v>7.8439712524414063E-3</v>
+      </c>
+      <c r="D119">
+        <v>19463.241307776985</v>
+      </c>
+      <c r="E119">
+        <v>4197.0189289632808</v>
+      </c>
+      <c r="F119">
+        <v>19005.335943220794</v>
+      </c>
+      <c r="G119">
+        <v>4.0568818672324996E-8</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A120">
+        <v>185.58030700683594</v>
+      </c>
+      <c r="B120">
+        <v>77.293461055255349</v>
+      </c>
+      <c r="C120">
+        <v>8.7976455688476563E-3</v>
+      </c>
+      <c r="D120">
+        <v>21354.949287213622</v>
+      </c>
+      <c r="E120">
+        <v>4697.1820456009964</v>
+      </c>
+      <c r="F120">
+        <v>20831.954778415518</v>
+      </c>
+      <c r="G120">
+        <v>4.116785305245025E-8</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A121">
+        <v>166.84437561035156</v>
+      </c>
+      <c r="B121">
+        <v>77.06412406467588</v>
+      </c>
+      <c r="C121">
+        <v>7.1287155151367188E-3</v>
+      </c>
+      <c r="D121">
+        <v>23411.586291542837</v>
+      </c>
+      <c r="E121">
+        <v>5240.9275878800172</v>
+      </c>
+      <c r="F121">
+        <v>22817.428661112423</v>
+      </c>
+      <c r="G121">
+        <v>4.180631218239855E-8</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A122">
+        <v>150</v>
+      </c>
+      <c r="B122">
+        <v>76.736719433583957</v>
+      </c>
+      <c r="C122">
+        <v>6.5565109252929688E-3</v>
+      </c>
+      <c r="D122">
+        <v>25657.995119333555</v>
+      </c>
+      <c r="E122">
+        <v>5886.6112899183472</v>
+      </c>
+      <c r="F122">
+        <v>24973.596478383934</v>
+      </c>
+      <c r="G122">
+        <v>4.2486189558814778E-8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BA31EA4-54FB-4B53-BD64-936367180BA0}">
   <dimension ref="A1:G132"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -3481,13 +6297,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5198625E-A763-4BDD-82AC-7EF979938D33}">
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E44286B-256D-46B8-8E3D-19D89F8AE9E7}">
   <dimension ref="A1:G132"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
@@ -6520,8 +9334,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54A6E8D4-0FA6-4162-B11B-C45649FC4159}">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57B7493A-6F5D-4C18-BDBE-9600A0D61E4D}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>